<commit_message>
Updated TC7 results Rev D
</commit_message>
<xml_diff>
--- a/Test Case - 7/TC7_Results_D.xlsx
+++ b/Test Case - 7/TC7_Results_D.xlsx
@@ -948,7 +948,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1508,8 +1528,8 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O10" sqref="O10"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,6 +2150,13 @@
       <c r="O13" s="3">
         <v>21.228000000000002</v>
       </c>
+      <c r="P13">
+        <f t="shared" ref="P13:P14" si="0">0.9*((O13-D13)^0.51)*((SQRT((M13-B13)^2+(N13-C13)^2)^(-0.35)))</f>
+        <v>4.2559362412849433</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -2177,6 +2204,13 @@
       <c r="O14" s="3">
         <v>21.228000000000002</v>
       </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>3.0340536432254828</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -3156,6 +3190,9 @@
       </c>
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
+      <c r="Q35" t="b">
+        <v>1</v>
+      </c>
       <c r="S35" t="s">
         <v>34</v>
       </c>
@@ -3200,6 +3237,9 @@
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
+      <c r="Q36" t="b">
+        <v>1</v>
+      </c>
       <c r="S36" t="s">
         <v>34</v>
       </c>
@@ -3244,6 +3284,9 @@
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
       <c r="O37" s="9"/>
+      <c r="Q37" t="b">
+        <v>1</v>
+      </c>
       <c r="S37" t="s">
         <v>34</v>
       </c>
@@ -3288,6 +3331,9 @@
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
+      <c r="Q38" t="b">
+        <v>1</v>
+      </c>
       <c r="S38" t="s">
         <v>34</v>
       </c>
@@ -3332,6 +3378,9 @@
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
+      <c r="Q39" t="b">
+        <v>1</v>
+      </c>
       <c r="S39" t="s">
         <v>34</v>
       </c>
@@ -3376,6 +3425,9 @@
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
       <c r="O40" s="9"/>
+      <c r="Q40" t="b">
+        <v>1</v>
+      </c>
       <c r="S40" t="s">
         <v>34</v>
       </c>
@@ -3420,6 +3472,9 @@
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
       <c r="O41" s="9"/>
+      <c r="Q41" t="b">
+        <v>1</v>
+      </c>
       <c r="S41" t="s">
         <v>34</v>
       </c>
@@ -3464,6 +3519,9 @@
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
       <c r="O42" s="9"/>
+      <c r="Q42" t="b">
+        <v>1</v>
+      </c>
       <c r="S42" t="s">
         <v>34</v>
       </c>
@@ -3508,6 +3566,9 @@
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
       <c r="O43" s="9"/>
+      <c r="Q43" t="b">
+        <v>1</v>
+      </c>
       <c r="S43" t="s">
         <v>34</v>
       </c>
@@ -3552,6 +3613,9 @@
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
       <c r="O44" s="9"/>
+      <c r="Q44" t="b">
+        <v>1</v>
+      </c>
       <c r="S44" t="s">
         <v>34</v>
       </c>
@@ -3596,6 +3660,9 @@
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
       <c r="O45" s="9"/>
+      <c r="Q45" t="b">
+        <v>1</v>
+      </c>
       <c r="S45" t="s">
         <v>34</v>
       </c>
@@ -3640,6 +3707,9 @@
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
       <c r="O46" s="9"/>
+      <c r="Q46" t="b">
+        <v>1</v>
+      </c>
       <c r="S46" t="s">
         <v>34</v>
       </c>
@@ -4429,14 +4499,22 @@
     <mergeCell ref="M1:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="L65 M3:M34 S35:S64">
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="41" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="42" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L65">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3">
     <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4444,23 +4522,23 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+  <conditionalFormatting sqref="Q29">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q29">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q12:Q14">
     <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4468,7 +4546,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q12">
+  <conditionalFormatting sqref="Q16">
     <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4476,7 +4554,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q16">
+  <conditionalFormatting sqref="Q17">
     <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4484,7 +4562,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17">
+  <conditionalFormatting sqref="Q23">
     <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4492,7 +4570,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q23">
+  <conditionalFormatting sqref="Q26">
     <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4500,19 +4578,19 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q26">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+  <conditionalFormatting sqref="Q22">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <conditionalFormatting sqref="Q35:Q46">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8757,26 +8835,26 @@
     <mergeCell ref="I1:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="R3:R63">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3:S63">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:U63">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>